<commit_message>
unselected and selected sheets
</commit_message>
<xml_diff>
--- a/Hackathon Coordinator/final 20.xlsx
+++ b/Hackathon Coordinator/final 20.xlsx
@@ -7,14 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Selected" sheetId="1" r:id="rId1"/>
+    <sheet name="Not Selected" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t>FULL NAME ( Team Leader )</t>
   </si>
@@ -266,6 +268,18 @@
   </si>
   <si>
     <t>sameer.patel201999@gmail.com</t>
+  </si>
+  <si>
+    <t>Mukul Singh Shekhawat</t>
+  </si>
+  <si>
+    <t>Rajasthan Institute of engineering and technology</t>
+  </si>
+  <si>
+    <t>Hack Warriors</t>
+  </si>
+  <si>
+    <t>mukulsinghshekhawat@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -989,4 +1003,489 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>